<commit_message>
New translations 口译量 1.26.xlsx(EN-US)
</commit_message>
<xml_diff>
--- a/en-US/口译量 1.26.xlsx
+++ b/en-US/口译量 1.26.xlsx
@@ -184,7 +184,96 @@
         <name val="微软雅黑"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">1010538930@qq. d </t>
+      <t xml:space="preserve">1010538930@qq. com </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>d</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">SX002-202-10193 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SX002-202-10193</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">山东大学 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>山东大学</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">淳于莎莎 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>淳于莎莎</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1538720819@qq. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1538720819@qq. com </t>
     </r>
     <r>
       <rPr>
@@ -204,16 +293,105 @@
         <name val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">SX002-202-10193 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>SX002-202-10193</t>
+      <t xml:space="preserve">SX002-202-10194 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SX002-202-10194</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">上海海事大学 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>上海海事大学</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">叶苏紫毓 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>叶苏紫毓</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">yeszyxm@foxmail. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">yeszyxm@foxmail. d </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>com</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">SX002-202-10195 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SX002-202-10195</t>
     </r>
   </si>
   <si>
@@ -244,36 +422,36 @@
         <name val="微软雅黑"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">淳于莎莎 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>淳于莎莎</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">1538720819@qq. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">1538720819@qq. d </t>
+      <t xml:space="preserve">王坤 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>王坤</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">363679074@qq. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">363679074@qq. com </t>
     </r>
     <r>
       <rPr>
@@ -293,165 +471,76 @@
         <name val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">SX002-202-10194 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>SX002-202-10194</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">上海海事大学 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海海事大学</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">叶苏紫毓 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>叶苏紫毓</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">yeszyxm@foxmail. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">yeszyxm@foxmail. com </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>d</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">SX002-202-10195 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>SX002-202-10195</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">山东大学 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>山东大学</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">王坤 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>王坤</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">363679074@qq. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">363679074@qq. d </t>
+      <t xml:space="preserve">SX002-202-10196 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SX002-202-10196</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">湖北大学 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>湖北大学</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">杨婕妤 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>杨婕妤</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">925012472@qq. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">sdf com </t>
     </r>
     <r>
       <rPr>
@@ -471,56 +560,36 @@
         <name val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">SX002-202-10196 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>SX002-202-10196</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">湖北大学 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>湖北大学</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">杨婕妤 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>杨婕妤</t>
+      <t xml:space="preserve">SX002-202-10197 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>df</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">df </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>上海大学</t>
     </r>
   </si>
   <si>
@@ -540,7 +609,27 @@
         <name val="微软雅黑"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">925012472@qq. d </t>
+      <t>李静</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">sdf </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">913543979@qq. d </t>
     </r>
     <r>
       <rPr>
@@ -560,76 +649,76 @@
         <name val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">df </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>SX002-202-10197</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">df </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上海大学</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">sdf </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>李静</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">sdf </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">913543979@qq. d </t>
+      <t xml:space="preserve">SX002-202-10198 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SX002-202-10198</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">宝鸡文理学院 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>宝鸡文理学院</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">赵子怡 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>赵子怡</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">869448674@qq. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">869448674@qq. d </t>
     </r>
     <r>
       <rPr>
@@ -649,76 +738,76 @@
         <name val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">SX002-202-10198 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>SX002-202-10198</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">宝鸡文理学院 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>宝鸡文理学院</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">赵子怡 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>赵子怡</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">869448674@qq. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">869448674@qq. d </t>
+      <t xml:space="preserve">SX002-202-10199 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SX002-202-10199</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">西南财经大学天府学院 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>西南财经大学天府学院</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">程亚舟 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>程亚舟</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">18782827811@163. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">18782827811@163. com </t>
     </r>
     <r>
       <rPr>
@@ -738,76 +827,76 @@
         <name val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">SX002-202-10199 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>SX002-202-10199</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">西南财经大学天府学院 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>西南财经大学天府学院</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">程亚舟 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>程亚舟</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">18782827811@163. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">18782827811@163. d </t>
+      <t xml:space="preserve">SX002-202-10200 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SX002-202-10200</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">西南科技大学 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>西南科技大学</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">邵佳 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>邵佳</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1051832884@qq. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1051832884@qq. d </t>
     </r>
     <r>
       <rPr>
@@ -827,95 +916,6 @@
         <name val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">SX002-202-10200 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>SX002-202-10200</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">西南科技大学 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>西南科技大学</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">邵佳 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>邵佳</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">1051832884@qq. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">1051832884@qq. com </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="微软雅黑"/>
-        <charset val="134"/>
-      </rPr>
-      <t>d</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">SX002-202-10201 </t>
     </r>
     <r>
@@ -985,7 +985,7 @@
         <name val="微软雅黑"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">437394119@qq. d </t>
+      <t xml:space="preserve">437394119@qq. com </t>
     </r>
     <r>
       <rPr>
@@ -1163,7 +1163,7 @@
         <name val="微软雅黑"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">1139893049@qq. d </t>
+      <t xml:space="preserve">1139893049@qq. com </t>
     </r>
     <r>
       <rPr>

</xml_diff>